<commit_message>
Better sensitivity graphs with k = 3.
</commit_message>
<xml_diff>
--- a/data/eeu_data.xlsx
+++ b/data/eeu_data.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mkh2/github/ReboundPaper2019/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mkh2/github/ReboundPaper2022/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33EE0249-4AB3-3E41-9B26-29A0409EFD3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{513B6989-9988-3246-A385-FF95253C4D5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="9080" xr2:uid="{7964B245-1BB5-784B-946F-34F7FEF70238}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="28800" windowHeight="9080" xr2:uid="{7964B245-1BB5-784B-946F-34F7FEF70238}"/>
   </bookViews>
   <sheets>
     <sheet name="EEU data" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -2936,12 +2936,1134 @@
         </r>
       </text>
     </comment>
+    <comment ref="G7" authorId="0" shapeId="0" xr:uid="{F02C9FA9-5124-1C4D-8C4A-EFF6EA33902E}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matthew Heun:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>MJ/gallon</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H7" authorId="0" shapeId="0" xr:uid="{942B85EE-DE94-5546-84FE-7A9129372F14}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matthew Heun:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>MJ/$</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J7" authorId="0" shapeId="0" xr:uid="{CAA7A6C8-4764-2347-AD95-949A1C1A3787}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matthew Heun:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>$/gal</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="N7" authorId="0" shapeId="0" xr:uid="{F3EF3C86-349A-2843-98C5-A337C21365A1}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matthew Heun:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>mi/gallon</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="O7" authorId="0" shapeId="0" xr:uid="{539A07E9-425F-0948-B2F9-BF3DC69024B5}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matthew Heun:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>mi/gallon</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="P7" authorId="0" shapeId="0" xr:uid="{36FC94B2-5124-9E47-A8ED-60189C2000D9}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matthew Heun:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>mi/yr</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="Q7" authorId="0" shapeId="0" xr:uid="{8CF48840-9560-3F45-9C0B-278A9A9CCE7A}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matthew Heun:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>$/year</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="R7" authorId="0" shapeId="0" xr:uid="{BA283CD6-9401-524A-A1FF-1ED7AE070966}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matthew Heun:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>$</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="S7" authorId="0" shapeId="0" xr:uid="{CE77C1C6-AC6F-8B43-9C2B-3C3779536172}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matthew Heun:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>year</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="T7" authorId="0" shapeId="0" xr:uid="{63BCA51A-5218-6B4A-AEBE-44F335CBAE4C}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matthew Heun:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>$</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="U7" authorId="0" shapeId="0" xr:uid="{3CF22B36-8CB7-A547-A065-FC8A32F784CD}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matthew Heun:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>year</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="V7" authorId="0" shapeId="0" xr:uid="{4C9A27A6-A338-4C42-833F-B78FCB97D194}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matthew Heun:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>$/year</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="W7" authorId="0" shapeId="0" xr:uid="{4664B37A-8190-044A-B078-C94A44149C24}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matthew Heun:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>$/year</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="X7" authorId="0" shapeId="0" xr:uid="{BDB90FF7-F1B8-5C43-84D0-692D5121C51D}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matthew Heun:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>MJ</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="Y7" authorId="0" shapeId="0" xr:uid="{A43D554B-0176-B942-93B4-273A673FFB4D}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matthew Heun:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>years</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="Z7" authorId="0" shapeId="0" xr:uid="{51A6AF1B-26A5-B844-9867-BFB9CDFFD6E0}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matthew Heun:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>MJ</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AA7" authorId="0" shapeId="0" xr:uid="{988C6C83-2782-3A48-8817-41D8728A25E3}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matthew Heun:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>years</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G8" authorId="0" shapeId="0" xr:uid="{7FFE18D2-A6E2-1343-8305-8561904C64C6}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matthew Heun:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>MJ/kW-hr</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H8" authorId="0" shapeId="0" xr:uid="{BD809D19-6CC8-C74A-A6A8-6317D12F2CF4}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matthew Heun:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>MJ/$</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J8" authorId="0" shapeId="0" xr:uid="{9BDE236B-7C2A-EA44-8C5A-F722CD943113}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matthew Heun:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>$/kW-hr</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="N8" authorId="0" shapeId="0" xr:uid="{2338F599-FCCF-0B41-95F6-B59B64312C5F}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matthew Heun:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>lm-hr/kW-hr</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="O8" authorId="0" shapeId="0" xr:uid="{AD170FB6-5306-F44E-BD01-1384C08BA3C0}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matthew Heun:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>lm-hr/kW-hr</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="P8" authorId="0" shapeId="0" xr:uid="{EF40C46C-CDB3-AD49-8844-34FD98A06203}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matthew Heun:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Lm-hr/yr</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="Q8" authorId="0" shapeId="0" xr:uid="{BCC1757E-D016-0F4C-9C4A-5AB130C9241A}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matthew Heun:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>$/year</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="R8" authorId="0" shapeId="0" xr:uid="{1430DDEA-5522-4441-811A-8F212A6E128E}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matthew Heun:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>$</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="S8" authorId="0" shapeId="0" xr:uid="{E4353DD3-5369-0F47-A8B5-3ADF3FC0EDBE}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matthew Heun:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>year</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="T8" authorId="0" shapeId="0" xr:uid="{03320AB5-156F-F44A-B983-16E48E375E62}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matthew Heun:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>$</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="U8" authorId="0" shapeId="0" xr:uid="{AC8EECA2-F3B6-824E-8B54-F30E7F2342A1}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matthew Heun:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>year</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="V8" authorId="0" shapeId="0" xr:uid="{C3D6566A-AC42-8142-A76F-CDEFCD09EB2C}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matthew Heun:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>$/year</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="W8" authorId="0" shapeId="0" xr:uid="{F94A9192-4DA6-C94D-AEA0-6AC29CE29A0F}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matthew Heun:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>$/year</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="X8" authorId="0" shapeId="0" xr:uid="{FC3408E6-2133-0240-AB0B-72191891EF1D}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matthew Heun:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>MJ</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="Y8" authorId="0" shapeId="0" xr:uid="{283C8A28-1ABF-9E49-AF62-4B8177DA20D6}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matthew Heun:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>years</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="Z8" authorId="0" shapeId="0" xr:uid="{ED48764E-0DE6-474B-99F1-B7FA628A3AC9}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matthew Heun:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>MJ</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AA8" authorId="0" shapeId="0" xr:uid="{0AB7DD1B-25CB-474D-B9DE-C96B24A9100E}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matthew Heun:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>years</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="43">
   <si>
     <t>Case</t>
   </si>
@@ -3065,6 +4187,12 @@
   <si>
     <t>Lamp - Germany</t>
   </si>
+  <si>
+    <t>Car (k = 3)</t>
+  </si>
+  <si>
+    <t>Lamp (k = 3)</t>
+  </si>
 </sst>
 </file>
 
@@ -3135,13 +4263,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3160,7 +4285,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2013 - 2022">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -3448,7 +4573,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -3456,10 +4581,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37C61C24-5EEE-2E43-8BFA-CC2DA9B61850}">
-  <dimension ref="A1:AA6"/>
+  <dimension ref="A1:AA8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3564,82 +4689,82 @@
       <c r="A2" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" t="s">
         <v>38</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" t="s">
         <v>30</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" t="s">
         <v>32</v>
       </c>
-      <c r="G2" s="3">
+      <c r="G2">
         <v>3.6</v>
       </c>
-      <c r="H2" s="2">
+      <c r="H2">
         <v>3.3893390630606501</v>
       </c>
-      <c r="I2" s="2">
+      <c r="I2">
         <v>1</v>
       </c>
-      <c r="J2" s="2">
+      <c r="J2">
         <v>0.12870000000000001</v>
       </c>
-      <c r="K2" s="2">
+      <c r="K2">
         <v>-0.4</v>
       </c>
-      <c r="L2" s="2">
+      <c r="L2">
         <v>1</v>
       </c>
-      <c r="M2" s="2">
+      <c r="M2">
         <v>1</v>
       </c>
-      <c r="N2" s="4">
+      <c r="N2" s="1">
         <v>8833.3333333333303</v>
       </c>
-      <c r="O2" s="2">
+      <c r="O2">
         <v>81800</v>
       </c>
-      <c r="P2" s="2">
+      <c r="P2">
         <v>580350</v>
       </c>
-      <c r="Q2" s="2">
+      <c r="Q2">
         <v>200</v>
       </c>
-      <c r="R2" s="2">
+      <c r="R2">
         <v>10</v>
       </c>
-      <c r="S2" s="2">
+      <c r="S2">
         <v>1.8</v>
       </c>
-      <c r="T2" s="2">
+      <c r="T2">
         <v>1</v>
       </c>
-      <c r="U2" s="2">
+      <c r="U2">
         <v>10</v>
       </c>
-      <c r="V2" s="2">
+      <c r="V2">
         <v>3</v>
       </c>
-      <c r="W2" s="2">
+      <c r="W2">
         <v>0</v>
       </c>
-      <c r="X2" s="2">
+      <c r="X2">
         <v>20</v>
       </c>
-      <c r="Y2" s="2">
+      <c r="Y2">
         <v>1</v>
       </c>
-      <c r="Z2" s="2">
+      <c r="Z2">
         <v>1</v>
       </c>
-      <c r="AA2" s="2">
+      <c r="AA2">
         <v>1</v>
       </c>
     </row>
@@ -3647,70 +4772,70 @@
       <c r="A3" t="s">
         <v>25</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" t="s">
         <v>26</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" t="s">
         <v>37</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" t="s">
         <v>29</v>
       </c>
-      <c r="G3" s="3">
+      <c r="G3">
         <v>126.62163000000001</v>
       </c>
-      <c r="H3" s="2">
+      <c r="H3">
         <v>3.2380660967337498</v>
       </c>
-      <c r="I3" s="2">
+      <c r="I3">
         <v>1</v>
       </c>
-      <c r="J3" s="2">
+      <c r="J3">
         <v>2.63</v>
       </c>
-      <c r="K3" s="2">
+      <c r="K3">
         <v>-0.2</v>
       </c>
-      <c r="L3" s="2">
+      <c r="L3">
         <v>1</v>
       </c>
-      <c r="M3" s="2">
+      <c r="M3">
         <v>1</v>
       </c>
-      <c r="N3" s="2">
+      <c r="N3">
         <v>25</v>
       </c>
-      <c r="O3" s="2">
+      <c r="O3">
         <v>42</v>
       </c>
-      <c r="P3" s="2">
+      <c r="P3">
         <v>12416</v>
       </c>
-      <c r="Q3" s="5">
+      <c r="Q3" s="2">
         <v>27929.825550000001</v>
       </c>
-      <c r="R3" s="2">
+      <c r="R3">
         <v>33446.43</v>
       </c>
-      <c r="S3" s="2">
+      <c r="S3">
         <v>7</v>
       </c>
       <c r="T3" s="1">
         <v>33037.919999999998</v>
       </c>
-      <c r="U3" s="2">
+      <c r="U3">
         <v>7</v>
       </c>
-      <c r="V3" s="5">
+      <c r="V3" s="2">
         <v>2730.84854</v>
       </c>
-      <c r="W3" s="5">
+      <c r="W3" s="2">
         <v>2709.6940300000001</v>
       </c>
       <c r="X3">
@@ -3730,82 +4855,82 @@
       <c r="A4" t="s">
         <v>25</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" t="s">
         <v>30</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="F4" t="s">
         <v>32</v>
       </c>
-      <c r="G4" s="3">
+      <c r="G4">
         <v>3.6</v>
       </c>
-      <c r="H4" s="2">
+      <c r="H4">
         <v>3.2380660967337498</v>
       </c>
-      <c r="I4" s="2">
+      <c r="I4">
         <v>1</v>
       </c>
-      <c r="J4" s="2">
+      <c r="J4">
         <v>0.12870000000000001</v>
       </c>
-      <c r="K4" s="2">
+      <c r="K4">
         <v>-0.4</v>
       </c>
-      <c r="L4" s="2">
+      <c r="L4">
         <v>1</v>
       </c>
-      <c r="M4" s="2">
+      <c r="M4">
         <v>1</v>
       </c>
-      <c r="N4" s="4">
+      <c r="N4" s="1">
         <v>8833.3333333333303</v>
       </c>
-      <c r="O4" s="2">
+      <c r="O4">
         <v>81800</v>
       </c>
-      <c r="P4" s="2">
+      <c r="P4">
         <v>580350</v>
       </c>
-      <c r="Q4" s="5">
+      <c r="Q4" s="2">
         <v>27929.825550000001</v>
       </c>
-      <c r="R4" s="2">
+      <c r="R4">
         <v>1.88</v>
       </c>
-      <c r="S4" s="2">
+      <c r="S4">
         <v>1.8</v>
       </c>
-      <c r="T4" s="2">
+      <c r="T4">
         <v>1.21</v>
       </c>
-      <c r="U4" s="2">
+      <c r="U4">
         <v>10</v>
       </c>
-      <c r="V4" s="2">
+      <c r="V4">
         <v>0</v>
       </c>
-      <c r="W4" s="2">
+      <c r="W4">
         <v>0</v>
       </c>
-      <c r="X4" s="2">
+      <c r="X4">
         <v>2.2000000000000002</v>
       </c>
-      <c r="Y4" s="2">
+      <c r="Y4">
         <v>1.8</v>
       </c>
-      <c r="Z4" s="2">
+      <c r="Z4">
         <v>6.5</v>
       </c>
-      <c r="AA4" s="2">
+      <c r="AA4">
         <v>10</v>
       </c>
     </row>
@@ -3813,70 +4938,70 @@
       <c r="A5" t="s">
         <v>25</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" t="s">
         <v>39</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E5" t="s">
         <v>37</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="F5" t="s">
         <v>29</v>
       </c>
-      <c r="G5" s="3">
+      <c r="G5">
         <v>126.62163000000001</v>
       </c>
-      <c r="H5" s="2">
+      <c r="H5">
         <v>3.2380660967337498</v>
       </c>
-      <c r="I5" s="2">
+      <c r="I5">
         <v>1</v>
       </c>
-      <c r="J5" s="2">
+      <c r="J5">
         <v>6.5</v>
       </c>
-      <c r="K5" s="2">
+      <c r="K5">
         <v>-0.2</v>
       </c>
-      <c r="L5" s="2">
+      <c r="L5">
         <v>1</v>
       </c>
-      <c r="M5" s="2">
+      <c r="M5">
         <v>1</v>
       </c>
-      <c r="N5" s="2">
+      <c r="N5">
         <v>25</v>
       </c>
-      <c r="O5" s="2">
+      <c r="O5">
         <v>42</v>
       </c>
-      <c r="P5" s="2">
+      <c r="P5">
         <v>12416</v>
       </c>
-      <c r="Q5" s="5">
+      <c r="Q5" s="2">
         <v>27929.825550000001</v>
       </c>
-      <c r="R5" s="2">
+      <c r="R5">
         <v>33446.43</v>
       </c>
-      <c r="S5" s="2">
+      <c r="S5">
         <v>7</v>
       </c>
       <c r="T5" s="1">
         <v>33037.919999999998</v>
       </c>
-      <c r="U5" s="2">
+      <c r="U5">
         <v>7</v>
       </c>
-      <c r="V5" s="5">
+      <c r="V5" s="2">
         <v>2730.84854</v>
       </c>
-      <c r="W5" s="5">
+      <c r="W5" s="2">
         <v>2709.6940300000001</v>
       </c>
       <c r="X5">
@@ -3896,82 +5021,248 @@
       <c r="A6" t="s">
         <v>25</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" t="s">
         <v>40</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="E6" t="s">
         <v>30</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="F6" t="s">
         <v>32</v>
       </c>
-      <c r="G6" s="3">
+      <c r="G6">
         <v>3.6</v>
       </c>
-      <c r="H6" s="2">
+      <c r="H6">
         <v>3.2380660967337498</v>
       </c>
-      <c r="I6" s="2">
+      <c r="I6">
         <v>1</v>
       </c>
-      <c r="J6" s="2">
+      <c r="J6">
         <v>0.36299999999999999</v>
       </c>
-      <c r="K6" s="2">
+      <c r="K6">
         <v>-0.4</v>
       </c>
-      <c r="L6" s="2">
+      <c r="L6">
         <v>1</v>
       </c>
-      <c r="M6" s="2">
+      <c r="M6">
         <v>1</v>
       </c>
-      <c r="N6" s="4">
+      <c r="N6" s="1">
         <v>8833.3333333333303</v>
       </c>
-      <c r="O6" s="2">
+      <c r="O6">
         <v>81800</v>
       </c>
-      <c r="P6" s="2">
+      <c r="P6">
         <v>580350</v>
       </c>
-      <c r="Q6" s="5">
+      <c r="Q6" s="2">
         <v>27929.825550000001</v>
       </c>
-      <c r="R6" s="2">
+      <c r="R6">
         <v>1.88</v>
       </c>
-      <c r="S6" s="2">
+      <c r="S6">
         <v>1.8</v>
       </c>
-      <c r="T6" s="2">
+      <c r="T6">
         <v>1.21</v>
       </c>
-      <c r="U6" s="2">
+      <c r="U6">
         <v>10</v>
       </c>
-      <c r="V6" s="2">
+      <c r="V6">
         <v>0</v>
       </c>
-      <c r="W6" s="2">
+      <c r="W6">
         <v>0</v>
       </c>
-      <c r="X6" s="2">
+      <c r="X6">
         <v>2.2000000000000002</v>
       </c>
-      <c r="Y6" s="2">
+      <c r="Y6">
         <v>1.8</v>
       </c>
-      <c r="Z6" s="2">
+      <c r="Z6">
         <v>6.5</v>
       </c>
-      <c r="AA6" s="2">
+      <c r="AA6">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" t="s">
+        <v>37</v>
+      </c>
+      <c r="F7" t="s">
+        <v>29</v>
+      </c>
+      <c r="G7">
+        <v>126.62163000000001</v>
+      </c>
+      <c r="H7">
+        <v>3.2380660967337498</v>
+      </c>
+      <c r="I7">
+        <v>3</v>
+      </c>
+      <c r="J7">
+        <v>2.63</v>
+      </c>
+      <c r="K7">
+        <v>-0.2</v>
+      </c>
+      <c r="L7">
+        <v>1</v>
+      </c>
+      <c r="M7">
+        <v>1</v>
+      </c>
+      <c r="N7">
+        <v>25</v>
+      </c>
+      <c r="O7">
+        <v>42</v>
+      </c>
+      <c r="P7">
+        <v>12416</v>
+      </c>
+      <c r="Q7" s="2">
+        <v>27929.825550000001</v>
+      </c>
+      <c r="R7">
+        <v>33446.43</v>
+      </c>
+      <c r="S7">
+        <v>7</v>
+      </c>
+      <c r="T7" s="1">
+        <v>33037.919999999998</v>
+      </c>
+      <c r="U7">
+        <v>7</v>
+      </c>
+      <c r="V7" s="2">
+        <v>2730.84854</v>
+      </c>
+      <c r="W7" s="2">
+        <v>2709.6940300000001</v>
+      </c>
+      <c r="X7">
+        <v>34000</v>
+      </c>
+      <c r="Y7">
+        <v>14</v>
+      </c>
+      <c r="Z7">
+        <v>40000</v>
+      </c>
+      <c r="AA7">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" t="s">
+        <v>42</v>
+      </c>
+      <c r="C8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" t="s">
+        <v>30</v>
+      </c>
+      <c r="F8" t="s">
+        <v>32</v>
+      </c>
+      <c r="G8">
+        <v>3.6</v>
+      </c>
+      <c r="H8">
+        <v>3.2380660967337498</v>
+      </c>
+      <c r="I8">
+        <v>3</v>
+      </c>
+      <c r="J8">
+        <v>0.12870000000000001</v>
+      </c>
+      <c r="K8">
+        <v>-0.4</v>
+      </c>
+      <c r="L8">
+        <v>1</v>
+      </c>
+      <c r="M8">
+        <v>1</v>
+      </c>
+      <c r="N8" s="1">
+        <v>8833.3333333333303</v>
+      </c>
+      <c r="O8">
+        <v>81800</v>
+      </c>
+      <c r="P8">
+        <v>580350</v>
+      </c>
+      <c r="Q8" s="2">
+        <v>27929.825550000001</v>
+      </c>
+      <c r="R8">
+        <v>1.88</v>
+      </c>
+      <c r="S8">
+        <v>1.8</v>
+      </c>
+      <c r="T8">
+        <v>1.21</v>
+      </c>
+      <c r="U8">
+        <v>10</v>
+      </c>
+      <c r="V8">
+        <v>0</v>
+      </c>
+      <c r="W8">
+        <v>0</v>
+      </c>
+      <c r="X8">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="Y8">
+        <v>1.8</v>
+      </c>
+      <c r="Z8">
+        <v>6.5</v>
+      </c>
+      <c r="AA8">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Change name of e_qs_ps_orig in Excel data sheet.
</commit_message>
<xml_diff>
--- a/data/eeu_data.xlsx
+++ b/data/eeu_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mkh2/github/ReboundPaper2022/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B6ADA5E-E654-114C-A218-2EC3ED3FB971}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80AFA438-C288-5E48-B9D3-F89AAD6B6318}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="28800" windowHeight="9080" xr2:uid="{7964B245-1BB5-784B-946F-34F7FEF70238}"/>
   </bookViews>
@@ -4120,9 +4120,6 @@
   </si>
   <si>
     <t>e_qo_M</t>
-  </si>
-  <si>
-    <t>e_qs_ps_UC</t>
   </si>
   <si>
     <t>t_own_orig</t>
@@ -4192,6 +4189,9 @@
   </si>
   <si>
     <t>Lamp (k = 3)</t>
+  </si>
+  <si>
+    <t>e_qs_ps_UC_orig</t>
   </si>
 </sst>
 </file>
@@ -4584,7 +4584,7 @@
   <dimension ref="A1:AA8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4604,7 +4604,7 @@
   <sheetData>
     <row r="1" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -4616,13 +4616,13 @@
         <v>2</v>
       </c>
       <c r="E1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H1" t="s">
         <v>11</v>
@@ -4631,10 +4631,10 @@
         <v>3</v>
       </c>
       <c r="J1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="K1" t="s">
-        <v>19</v>
+        <v>42</v>
       </c>
       <c r="L1" t="s">
         <v>17</v>
@@ -4643,10 +4643,10 @@
         <v>18</v>
       </c>
       <c r="N1" t="s">
+        <v>33</v>
+      </c>
+      <c r="O1" t="s">
         <v>34</v>
-      </c>
-      <c r="O1" t="s">
-        <v>35</v>
       </c>
       <c r="P1" t="s">
         <v>4</v>
@@ -4658,13 +4658,13 @@
         <v>13</v>
       </c>
       <c r="S1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="T1" t="s">
         <v>14</v>
       </c>
       <c r="U1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="V1" t="s">
         <v>5</v>
@@ -4676,21 +4676,21 @@
         <v>15</v>
       </c>
       <c r="Y1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="Z1" t="s">
         <v>16</v>
       </c>
       <c r="AA1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C2" t="s">
         <v>9</v>
@@ -4699,10 +4699,10 @@
         <v>10</v>
       </c>
       <c r="E2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G2">
         <v>3.6</v>
@@ -4770,10 +4770,10 @@
     </row>
     <row r="3" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" t="s">
         <v>25</v>
-      </c>
-      <c r="B3" t="s">
-        <v>26</v>
       </c>
       <c r="C3" t="s">
         <v>7</v>
@@ -4782,10 +4782,10 @@
         <v>8</v>
       </c>
       <c r="E3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G3">
         <v>126.62163000000001</v>
@@ -4853,10 +4853,10 @@
     </row>
     <row r="4" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C4" t="s">
         <v>9</v>
@@ -4865,10 +4865,10 @@
         <v>10</v>
       </c>
       <c r="E4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G4">
         <v>3.6</v>
@@ -4936,10 +4936,10 @@
     </row>
     <row r="5" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C5" t="s">
         <v>7</v>
@@ -4948,10 +4948,10 @@
         <v>8</v>
       </c>
       <c r="E5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G5">
         <v>126.62163000000001</v>
@@ -5019,10 +5019,10 @@
     </row>
     <row r="6" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C6" t="s">
         <v>9</v>
@@ -5031,10 +5031,10 @@
         <v>10</v>
       </c>
       <c r="E6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G6">
         <v>3.6</v>
@@ -5102,10 +5102,10 @@
     </row>
     <row r="7" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C7" t="s">
         <v>7</v>
@@ -5114,10 +5114,10 @@
         <v>8</v>
       </c>
       <c r="E7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G7">
         <v>126.62163000000001</v>
@@ -5185,10 +5185,10 @@
     </row>
     <row r="8" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C8" t="s">
         <v>9</v>
@@ -5197,10 +5197,10 @@
         <v>10</v>
       </c>
       <c r="E8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G8">
         <v>3.6</v>

</xml_diff>

<commit_message>
Fix units in stages tables.
</commit_message>
<xml_diff>
--- a/data/eeu_data.xlsx
+++ b/data/eeu_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mkh2/github/ReboundPaper2022/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80AFA438-C288-5E48-B9D3-F89AAD6B6318}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{547E0499-0657-7449-A519-8D571828C1BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="28800" windowHeight="9080" xr2:uid="{7964B245-1BB5-784B-946F-34F7FEF70238}"/>
   </bookViews>
@@ -28,6 +28,8 @@
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Matthew Heun</author>
+    <author>tc={330A8BDF-B9E8-FC4D-9703-7960C268D81C}</author>
+    <author>tc={2F78887D-BE5A-1D4A-8E64-14B7D80057C4}</author>
   </authors>
   <commentList>
     <comment ref="E1" authorId="0" shapeId="0" xr:uid="{177A5939-9C5C-134F-8638-CA4D7AC90D6E}">
@@ -127,6 +129,22 @@
           </rPr>
           <t>This unit conversion factor translates from energy engineering units to MJ.</t>
         </r>
+      </text>
+    </comment>
+    <comment ref="E2" authorId="1" shapeId="0" xr:uid="{330A8BDF-B9E8-FC4D-9703-7960C268D81C}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    \lmhr is a macro in the ReboundPaper2022 repository hat expands into the right thing (lm-hr but with a dot)</t>
+      </text>
+    </comment>
+    <comment ref="F2" authorId="2" shapeId="0" xr:uid="{2F78887D-BE5A-1D4A-8E64-14B7D80057C4}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    \kWhr is a macro in the ReboundTools2022 repository that expands into the right thing (kW-hr but with a dot)</t>
       </text>
     </comment>
     <comment ref="G2" authorId="0" shapeId="0" xr:uid="{249B88D5-8C45-2F49-B897-04C08FC94B9A}">
@@ -4152,13 +4170,7 @@
     <t>gal</t>
   </si>
   <si>
-    <t>lm-hr</t>
-  </si>
-  <si>
     <t>service_unit</t>
-  </si>
-  <si>
-    <t>kW-hr</t>
   </si>
   <si>
     <t>p_E_engr_units</t>
@@ -4192,6 +4204,12 @@
   </si>
   <si>
     <t>e_qs_ps_UC_orig</t>
+  </si>
+  <si>
+    <t>\lmhr</t>
+  </si>
+  <si>
+    <t>\kWhr</t>
   </si>
 </sst>
 </file>
@@ -4282,6 +4300,12 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="Matthew Heun" id="{B33520C4-052D-C94A-99DA-F069052A89CB}" userId="S::mkh2@calvin.edu::790ed012-1f73-4faf-8a49-cb7986d89887" providerId="AD"/>
+</personList>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4579,12 +4603,23 @@
 </a:theme>
 </file>
 
+<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="E2" dT="2023-01-08T19:34:49.71" personId="{B33520C4-052D-C94A-99DA-F069052A89CB}" id="{330A8BDF-B9E8-FC4D-9703-7960C268D81C}">
+    <text>\lmhr is a macro in the ReboundPaper2022 repository hat expands into the right thing (lm-hr but with a dot)</text>
+  </threadedComment>
+  <threadedComment ref="F2" dT="2023-01-08T19:35:22.94" personId="{B33520C4-052D-C94A-99DA-F069052A89CB}" id="{2F78887D-BE5A-1D4A-8E64-14B7D80057C4}">
+    <text>\kWhr is a macro in the ReboundTools2022 repository that expands into the right thing (kW-hr but with a dot)</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37C61C24-5EEE-2E43-8BFA-CC2DA9B61850}">
   <dimension ref="A1:AA8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4616,13 +4651,13 @@
         <v>2</v>
       </c>
       <c r="E1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F1" t="s">
         <v>27</v>
       </c>
       <c r="G1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="H1" t="s">
         <v>11</v>
@@ -4631,10 +4666,10 @@
         <v>3</v>
       </c>
       <c r="J1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="K1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="L1" t="s">
         <v>17</v>
@@ -4643,10 +4678,10 @@
         <v>18</v>
       </c>
       <c r="N1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="O1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="P1" t="s">
         <v>4</v>
@@ -4690,7 +4725,7 @@
         <v>24</v>
       </c>
       <c r="B2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C2" t="s">
         <v>9</v>
@@ -4699,10 +4734,10 @@
         <v>10</v>
       </c>
       <c r="E2" t="s">
-        <v>29</v>
+        <v>41</v>
       </c>
       <c r="F2" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="G2">
         <v>3.6</v>
@@ -4782,7 +4817,7 @@
         <v>8</v>
       </c>
       <c r="E3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F3" t="s">
         <v>28</v>
@@ -4865,10 +4900,10 @@
         <v>10</v>
       </c>
       <c r="E4" t="s">
-        <v>29</v>
+        <v>41</v>
       </c>
       <c r="F4" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="G4">
         <v>3.6</v>
@@ -4939,7 +4974,7 @@
         <v>24</v>
       </c>
       <c r="B5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C5" t="s">
         <v>7</v>
@@ -4948,7 +4983,7 @@
         <v>8</v>
       </c>
       <c r="E5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F5" t="s">
         <v>28</v>
@@ -5022,7 +5057,7 @@
         <v>24</v>
       </c>
       <c r="B6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C6" t="s">
         <v>9</v>
@@ -5031,10 +5066,10 @@
         <v>10</v>
       </c>
       <c r="E6" t="s">
-        <v>29</v>
+        <v>41</v>
       </c>
       <c r="F6" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="G6">
         <v>3.6</v>
@@ -5105,7 +5140,7 @@
         <v>24</v>
       </c>
       <c r="B7" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C7" t="s">
         <v>7</v>
@@ -5114,7 +5149,7 @@
         <v>8</v>
       </c>
       <c r="E7" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F7" t="s">
         <v>28</v>
@@ -5188,7 +5223,7 @@
         <v>24</v>
       </c>
       <c r="B8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C8" t="s">
         <v>9</v>
@@ -5197,10 +5232,10 @@
         <v>10</v>
       </c>
       <c r="E8" t="s">
-        <v>29</v>
+        <v>41</v>
       </c>
       <c r="F8" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="G8">
         <v>3.6</v>

</xml_diff>

<commit_message>
Working on updated car case parameters
</commit_message>
<xml_diff>
--- a/data/eeu_data.xlsx
+++ b/data/eeu_data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mkh2/github/ReboundPaper2022/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4556A4B-AD1D-BD41-887E-D7BE43382033}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8B3EACF-5981-3E4D-BE24-20C6C2BA0E87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="28800" windowHeight="9080" xr2:uid="{7964B245-1BB5-784B-946F-34F7FEF70238}"/>
   </bookViews>
@@ -19,6 +19,17 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -1364,7 +1375,6 @@
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
-            <scheme val="minor"/>
           </rPr>
           <t>Disposal cost at end of life, $</t>
         </r>
@@ -4502,12 +4512,18 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -4522,10 +4538,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="4" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4860,7 +4878,10 @@
   <dimension ref="A1:AD8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Z3" sqref="Z3:Z8"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="S2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="E1" sqref="E1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="Y10" sqref="Y10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5130,17 +5151,17 @@
       <c r="V3">
         <v>7</v>
       </c>
-      <c r="W3" s="2">
-        <v>2730.84854</v>
-      </c>
-      <c r="X3" s="2">
-        <v>2709.6940300000001</v>
-      </c>
-      <c r="Y3">
-        <v>0</v>
-      </c>
-      <c r="Z3">
-        <v>0</v>
+      <c r="W3" s="3">
+        <v>5000</v>
+      </c>
+      <c r="X3" s="3">
+        <v>5000</v>
+      </c>
+      <c r="Y3" s="4">
+        <v>-300</v>
+      </c>
+      <c r="Z3" s="4">
+        <v>-300</v>
       </c>
       <c r="AA3">
         <v>34000</v>

</xml_diff>

<commit_message>
Updating eeu_data to match PEB results
</commit_message>
<xml_diff>
--- a/data/eeu_data.xlsx
+++ b/data/eeu_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mkh2/github/ReboundPaper2022/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8B3EACF-5981-3E4D-BE24-20C6C2BA0E87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE2B2D7E-A3FA-5642-8DCF-F97BEE3FEEA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="28800" windowHeight="9080" xr2:uid="{7964B245-1BB5-784B-946F-34F7FEF70238}"/>
   </bookViews>
@@ -489,40 +489,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="T2" authorId="1" shapeId="0" xr:uid="{0DA7397A-F905-1A43-8CD3-0EC341171AE9}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Matthew Heun:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>year</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="U2" authorId="1" shapeId="0" xr:uid="{267C6984-34ED-C149-AA4B-45EDCF917BC6}">
+    <comment ref="T2" authorId="1" shapeId="0" xr:uid="{267C6984-34ED-C149-AA4B-45EDCF917BC6}">
       <text>
         <r>
           <rPr>
@@ -555,40 +522,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="V2" authorId="1" shapeId="0" xr:uid="{E4325DB6-2B17-E64E-B67E-4039ECC386FD}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Matthew Heun:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>year</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="W2" authorId="1" shapeId="0" xr:uid="{9B9C601E-788F-B24F-8483-064FAE23D2C7}">
+    <comment ref="U2" authorId="1" shapeId="0" xr:uid="{9B9C601E-788F-B24F-8483-064FAE23D2C7}">
       <text>
         <r>
           <rPr>
@@ -621,7 +555,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="X2" authorId="1" shapeId="0" xr:uid="{0B3A1821-343E-A046-84C1-A43EE53EE234}">
+    <comment ref="V2" authorId="1" shapeId="0" xr:uid="{0B3A1821-343E-A046-84C1-A43EE53EE234}">
       <text>
         <r>
           <rPr>
@@ -654,7 +588,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Y2" authorId="1" shapeId="0" xr:uid="{00D12488-AD0D-F14E-9A3F-6905E9D3286A}">
+    <comment ref="W2" authorId="1" shapeId="0" xr:uid="{00D12488-AD0D-F14E-9A3F-6905E9D3286A}">
       <text>
         <r>
           <rPr>
@@ -687,7 +621,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Z2" authorId="1" shapeId="0" xr:uid="{39352CD7-2821-2446-9594-6E2AAAC0C6C6}">
+    <comment ref="X2" authorId="1" shapeId="0" xr:uid="{39352CD7-2821-2446-9594-6E2AAAC0C6C6}">
       <text>
         <r>
           <rPr>
@@ -720,7 +654,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AA2" authorId="1" shapeId="0" xr:uid="{BA077B63-1D59-DE46-8B9E-A045A76E395D}">
+    <comment ref="Y2" authorId="1" shapeId="0" xr:uid="{BA077B63-1D59-DE46-8B9E-A045A76E395D}">
       <text>
         <r>
           <rPr>
@@ -753,7 +687,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AB2" authorId="1" shapeId="0" xr:uid="{C80E81A5-BB38-8344-A6B2-AA6FA5F9F335}">
+    <comment ref="Z2" authorId="1" shapeId="0" xr:uid="{C80E81A5-BB38-8344-A6B2-AA6FA5F9F335}">
       <text>
         <r>
           <rPr>
@@ -786,7 +720,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AC2" authorId="1" shapeId="0" xr:uid="{B1142E16-9D5A-F947-8B83-E5ADE08AC501}">
+    <comment ref="AA2" authorId="1" shapeId="0" xr:uid="{B1142E16-9D5A-F947-8B83-E5ADE08AC501}">
       <text>
         <r>
           <rPr>
@@ -819,7 +753,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AD2" authorId="1" shapeId="0" xr:uid="{5FC48D65-41E9-E442-8F22-B5DAACE45501}">
+    <comment ref="AB2" authorId="1" shapeId="0" xr:uid="{5FC48D65-41E9-E442-8F22-B5DAACE45501}">
       <text>
         <r>
           <rPr>
@@ -1149,40 +1083,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="T3" authorId="1" shapeId="0" xr:uid="{C60C194C-E6D8-714B-8103-E2256CEE5592}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Matthew Heun:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>year</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="U3" authorId="1" shapeId="0" xr:uid="{FF3DF81E-1DB0-BC43-B287-7EE6D75FE27A}">
+    <comment ref="T3" authorId="1" shapeId="0" xr:uid="{FF3DF81E-1DB0-BC43-B287-7EE6D75FE27A}">
       <text>
         <r>
           <rPr>
@@ -1215,40 +1116,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="V3" authorId="1" shapeId="0" xr:uid="{518F164D-FDCC-E54D-B2DF-8F453ECB1431}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Matthew Heun:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>year</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="W3" authorId="1" shapeId="0" xr:uid="{B7D79E05-3555-1641-A199-607AD17F3A98}">
+    <comment ref="U3" authorId="1" shapeId="0" xr:uid="{B7D79E05-3555-1641-A199-607AD17F3A98}">
       <text>
         <r>
           <rPr>
@@ -1281,7 +1149,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="X3" authorId="1" shapeId="0" xr:uid="{EB6F1D42-7F43-8642-AA41-BBF50B143386}">
+    <comment ref="V3" authorId="1" shapeId="0" xr:uid="{EB6F1D42-7F43-8642-AA41-BBF50B143386}">
       <text>
         <r>
           <rPr>
@@ -1314,7 +1182,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Y3" authorId="1" shapeId="0" xr:uid="{4D851FFD-F26D-D848-91D4-8046D752B86C}">
+    <comment ref="W3" authorId="1" shapeId="0" xr:uid="{4D851FFD-F26D-D848-91D4-8046D752B86C}">
       <text>
         <r>
           <rPr>
@@ -1347,7 +1215,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Z3" authorId="1" shapeId="0" xr:uid="{3EC860A8-0F07-DB40-B72D-F233361D3394}">
+    <comment ref="X3" authorId="1" shapeId="0" xr:uid="{3EC860A8-0F07-DB40-B72D-F233361D3394}">
       <text>
         <r>
           <rPr>
@@ -1380,7 +1248,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AA3" authorId="1" shapeId="0" xr:uid="{AE95BD72-263E-7640-8218-827926A6729F}">
+    <comment ref="Y3" authorId="1" shapeId="0" xr:uid="{AE95BD72-263E-7640-8218-827926A6729F}">
       <text>
         <r>
           <rPr>
@@ -1413,7 +1281,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AB3" authorId="1" shapeId="0" xr:uid="{047D8163-FB8F-4246-99B2-595867513897}">
+    <comment ref="Z3" authorId="1" shapeId="0" xr:uid="{047D8163-FB8F-4246-99B2-595867513897}">
       <text>
         <r>
           <rPr>
@@ -1446,7 +1314,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AC3" authorId="1" shapeId="0" xr:uid="{7BA8270B-AFA1-CD4D-B70B-0C32B322B130}">
+    <comment ref="AA3" authorId="1" shapeId="0" xr:uid="{7BA8270B-AFA1-CD4D-B70B-0C32B322B130}">
       <text>
         <r>
           <rPr>
@@ -1479,7 +1347,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AD3" authorId="1" shapeId="0" xr:uid="{726EEEB5-AC80-0243-B610-FEFA2F34A1EB}">
+    <comment ref="AB3" authorId="1" shapeId="0" xr:uid="{726EEEB5-AC80-0243-B610-FEFA2F34A1EB}">
       <text>
         <r>
           <rPr>
@@ -1776,40 +1644,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="T4" authorId="1" shapeId="0" xr:uid="{DDB014C5-A2CC-FC47-AB30-9F51ABE81900}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Matthew Heun:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>year</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="U4" authorId="1" shapeId="0" xr:uid="{F75309F3-B254-6B42-ACF3-EB7B62070C9A}">
+    <comment ref="T4" authorId="1" shapeId="0" xr:uid="{F75309F3-B254-6B42-ACF3-EB7B62070C9A}">
       <text>
         <r>
           <rPr>
@@ -1842,40 +1677,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="V4" authorId="1" shapeId="0" xr:uid="{FCC815E5-11DC-7845-9B83-107B9BB0833E}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Matthew Heun:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>year</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="W4" authorId="1" shapeId="0" xr:uid="{8841F362-90D3-8C4C-AC8E-5C78D027A50A}">
+    <comment ref="U4" authorId="1" shapeId="0" xr:uid="{8841F362-90D3-8C4C-AC8E-5C78D027A50A}">
       <text>
         <r>
           <rPr>
@@ -1908,7 +1710,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="X4" authorId="1" shapeId="0" xr:uid="{99786566-807D-2141-B3D8-EC9C23CFBD56}">
+    <comment ref="V4" authorId="1" shapeId="0" xr:uid="{99786566-807D-2141-B3D8-EC9C23CFBD56}">
       <text>
         <r>
           <rPr>
@@ -1941,7 +1743,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AA4" authorId="1" shapeId="0" xr:uid="{4DF8FA29-C568-E543-91D3-01421B5896B3}">
+    <comment ref="Y4" authorId="1" shapeId="0" xr:uid="{4DF8FA29-C568-E543-91D3-01421B5896B3}">
       <text>
         <r>
           <rPr>
@@ -1974,7 +1776,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AB4" authorId="1" shapeId="0" xr:uid="{2881D54C-6A08-2541-9F80-637268D2285C}">
+    <comment ref="Z4" authorId="1" shapeId="0" xr:uid="{2881D54C-6A08-2541-9F80-637268D2285C}">
       <text>
         <r>
           <rPr>
@@ -2007,7 +1809,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AC4" authorId="1" shapeId="0" xr:uid="{35E3A805-B627-0643-B8CC-944CC619506C}">
+    <comment ref="AA4" authorId="1" shapeId="0" xr:uid="{35E3A805-B627-0643-B8CC-944CC619506C}">
       <text>
         <r>
           <rPr>
@@ -2040,7 +1842,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AD4" authorId="1" shapeId="0" xr:uid="{8C08D8AD-E643-AD46-9778-37D19F8C80AE}">
+    <comment ref="AB4" authorId="1" shapeId="0" xr:uid="{8C08D8AD-E643-AD46-9778-37D19F8C80AE}">
       <text>
         <r>
           <rPr>
@@ -2337,40 +2139,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="T5" authorId="1" shapeId="0" xr:uid="{F49AB31C-960A-9547-9947-81A4B07608EE}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Matthew Heun:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>year</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="U5" authorId="1" shapeId="0" xr:uid="{4CBDBD7B-5BF2-E043-AA1C-5E1E1FF54EA9}">
+    <comment ref="T5" authorId="1" shapeId="0" xr:uid="{4CBDBD7B-5BF2-E043-AA1C-5E1E1FF54EA9}">
       <text>
         <r>
           <rPr>
@@ -2403,40 +2172,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="V5" authorId="1" shapeId="0" xr:uid="{8FF7AA45-0FBB-D64A-905B-F3B136F66C54}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Matthew Heun:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>year</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="W5" authorId="1" shapeId="0" xr:uid="{5E184648-FE58-B641-A34A-0ADD6FDF7F5F}">
+    <comment ref="U5" authorId="1" shapeId="0" xr:uid="{5E184648-FE58-B641-A34A-0ADD6FDF7F5F}">
       <text>
         <r>
           <rPr>
@@ -2469,7 +2205,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="X5" authorId="1" shapeId="0" xr:uid="{F56383BC-5696-044D-B109-42EC8262A1B4}">
+    <comment ref="V5" authorId="1" shapeId="0" xr:uid="{F56383BC-5696-044D-B109-42EC8262A1B4}">
       <text>
         <r>
           <rPr>
@@ -2502,7 +2238,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AA5" authorId="1" shapeId="0" xr:uid="{19D45708-CD7B-8247-BCE0-4E84383FEA96}">
+    <comment ref="Y5" authorId="1" shapeId="0" xr:uid="{19D45708-CD7B-8247-BCE0-4E84383FEA96}">
       <text>
         <r>
           <rPr>
@@ -2535,7 +2271,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AB5" authorId="1" shapeId="0" xr:uid="{282B7987-5567-E04A-8D32-E930CE7FA9C8}">
+    <comment ref="Z5" authorId="1" shapeId="0" xr:uid="{282B7987-5567-E04A-8D32-E930CE7FA9C8}">
       <text>
         <r>
           <rPr>
@@ -2568,7 +2304,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AC5" authorId="1" shapeId="0" xr:uid="{E437800C-4DFD-AC41-8098-B5A4689AC3FF}">
+    <comment ref="AA5" authorId="1" shapeId="0" xr:uid="{E437800C-4DFD-AC41-8098-B5A4689AC3FF}">
       <text>
         <r>
           <rPr>
@@ -2601,7 +2337,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AD5" authorId="1" shapeId="0" xr:uid="{EDC7D713-6DDC-4A42-9B2D-55BE182647AF}">
+    <comment ref="AB5" authorId="1" shapeId="0" xr:uid="{EDC7D713-6DDC-4A42-9B2D-55BE182647AF}">
       <text>
         <r>
           <rPr>
@@ -2899,40 +2635,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="T6" authorId="1" shapeId="0" xr:uid="{BAF76ADD-69BA-2848-8289-DB107E768723}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Matthew Heun:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>year</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="U6" authorId="1" shapeId="0" xr:uid="{6557DCD5-3C86-1F41-A9DA-B746D947FAFB}">
+    <comment ref="T6" authorId="1" shapeId="0" xr:uid="{6557DCD5-3C86-1F41-A9DA-B746D947FAFB}">
       <text>
         <r>
           <rPr>
@@ -2965,40 +2668,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="V6" authorId="1" shapeId="0" xr:uid="{0328129B-43CF-8643-8219-AE7727F6A1E9}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Matthew Heun:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>year</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="W6" authorId="1" shapeId="0" xr:uid="{41960BAA-D066-F445-9D8F-B1974FDBE9E9}">
+    <comment ref="U6" authorId="1" shapeId="0" xr:uid="{41960BAA-D066-F445-9D8F-B1974FDBE9E9}">
       <text>
         <r>
           <rPr>
@@ -3031,7 +2701,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="X6" authorId="1" shapeId="0" xr:uid="{60240E64-7507-0743-978C-D1A72091792A}">
+    <comment ref="V6" authorId="1" shapeId="0" xr:uid="{60240E64-7507-0743-978C-D1A72091792A}">
       <text>
         <r>
           <rPr>
@@ -3064,7 +2734,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AA6" authorId="1" shapeId="0" xr:uid="{A1F0BA58-1501-8F4C-9FE7-A0A402682788}">
+    <comment ref="Y6" authorId="1" shapeId="0" xr:uid="{A1F0BA58-1501-8F4C-9FE7-A0A402682788}">
       <text>
         <r>
           <rPr>
@@ -3097,7 +2767,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AB6" authorId="1" shapeId="0" xr:uid="{0539EDFB-7118-4045-B941-10E5FF9B703A}">
+    <comment ref="Z6" authorId="1" shapeId="0" xr:uid="{0539EDFB-7118-4045-B941-10E5FF9B703A}">
       <text>
         <r>
           <rPr>
@@ -3130,7 +2800,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AC6" authorId="1" shapeId="0" xr:uid="{9FC449E1-E514-FB42-B0AC-C35D6A7AF47E}">
+    <comment ref="AA6" authorId="1" shapeId="0" xr:uid="{9FC449E1-E514-FB42-B0AC-C35D6A7AF47E}">
       <text>
         <r>
           <rPr>
@@ -3163,7 +2833,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AD6" authorId="1" shapeId="0" xr:uid="{8F842682-DEE9-5E41-A460-BED7BB769A84}">
+    <comment ref="AB6" authorId="1" shapeId="0" xr:uid="{8F842682-DEE9-5E41-A460-BED7BB769A84}">
       <text>
         <r>
           <rPr>
@@ -3460,40 +3130,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="T7" authorId="1" shapeId="0" xr:uid="{CE77C1C6-AC6F-8B43-9C2B-3C3779536172}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Matthew Heun:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>year</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="U7" authorId="1" shapeId="0" xr:uid="{63BCA51A-5218-6B4A-AEBE-44F335CBAE4C}">
+    <comment ref="T7" authorId="1" shapeId="0" xr:uid="{63BCA51A-5218-6B4A-AEBE-44F335CBAE4C}">
       <text>
         <r>
           <rPr>
@@ -3526,40 +3163,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="V7" authorId="1" shapeId="0" xr:uid="{3CF22B36-8CB7-A547-A065-FC8A32F784CD}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Matthew Heun:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>year</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="W7" authorId="1" shapeId="0" xr:uid="{4C9A27A6-A338-4C42-833F-B78FCB97D194}">
+    <comment ref="U7" authorId="1" shapeId="0" xr:uid="{4C9A27A6-A338-4C42-833F-B78FCB97D194}">
       <text>
         <r>
           <rPr>
@@ -3592,7 +3196,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="X7" authorId="1" shapeId="0" xr:uid="{4664B37A-8190-044A-B078-C94A44149C24}">
+    <comment ref="V7" authorId="1" shapeId="0" xr:uid="{4664B37A-8190-044A-B078-C94A44149C24}">
       <text>
         <r>
           <rPr>
@@ -3625,7 +3229,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AA7" authorId="1" shapeId="0" xr:uid="{BDB90FF7-F1B8-5C43-84D0-692D5121C51D}">
+    <comment ref="Y7" authorId="1" shapeId="0" xr:uid="{BDB90FF7-F1B8-5C43-84D0-692D5121C51D}">
       <text>
         <r>
           <rPr>
@@ -3658,7 +3262,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AB7" authorId="1" shapeId="0" xr:uid="{A43D554B-0176-B942-93B4-273A673FFB4D}">
+    <comment ref="Z7" authorId="1" shapeId="0" xr:uid="{A43D554B-0176-B942-93B4-273A673FFB4D}">
       <text>
         <r>
           <rPr>
@@ -3691,7 +3295,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AC7" authorId="1" shapeId="0" xr:uid="{51A6AF1B-26A5-B844-9867-BFB9CDFFD6E0}">
+    <comment ref="AA7" authorId="1" shapeId="0" xr:uid="{51A6AF1B-26A5-B844-9867-BFB9CDFFD6E0}">
       <text>
         <r>
           <rPr>
@@ -3724,7 +3328,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AD7" authorId="1" shapeId="0" xr:uid="{988C6C83-2782-3A48-8817-41D8728A25E3}">
+    <comment ref="AB7" authorId="1" shapeId="0" xr:uid="{988C6C83-2782-3A48-8817-41D8728A25E3}">
       <text>
         <r>
           <rPr>
@@ -4021,40 +3625,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="T8" authorId="1" shapeId="0" xr:uid="{E4353DD3-5369-0F47-A8B5-3ADF3FC0EDBE}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Matthew Heun:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>year</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="U8" authorId="1" shapeId="0" xr:uid="{03320AB5-156F-F44A-B983-16E48E375E62}">
+    <comment ref="T8" authorId="1" shapeId="0" xr:uid="{03320AB5-156F-F44A-B983-16E48E375E62}">
       <text>
         <r>
           <rPr>
@@ -4087,40 +3658,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="V8" authorId="1" shapeId="0" xr:uid="{AC8EECA2-F3B6-824E-8B54-F30E7F2342A1}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Matthew Heun:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>year</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="W8" authorId="1" shapeId="0" xr:uid="{C3D6566A-AC42-8142-A76F-CDEFCD09EB2C}">
+    <comment ref="U8" authorId="1" shapeId="0" xr:uid="{C3D6566A-AC42-8142-A76F-CDEFCD09EB2C}">
       <text>
         <r>
           <rPr>
@@ -4153,7 +3691,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="X8" authorId="1" shapeId="0" xr:uid="{F94A9192-4DA6-C94D-AEA0-6AC29CE29A0F}">
+    <comment ref="V8" authorId="1" shapeId="0" xr:uid="{F94A9192-4DA6-C94D-AEA0-6AC29CE29A0F}">
       <text>
         <r>
           <rPr>
@@ -4186,7 +3724,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AA8" authorId="1" shapeId="0" xr:uid="{FC3408E6-2133-0240-AB0B-72191891EF1D}">
+    <comment ref="Y8" authorId="1" shapeId="0" xr:uid="{FC3408E6-2133-0240-AB0B-72191891EF1D}">
       <text>
         <r>
           <rPr>
@@ -4219,7 +3757,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AB8" authorId="1" shapeId="0" xr:uid="{283C8A28-1ABF-9E49-AF62-4B8177DA20D6}">
+    <comment ref="Z8" authorId="1" shapeId="0" xr:uid="{283C8A28-1ABF-9E49-AF62-4B8177DA20D6}">
       <text>
         <r>
           <rPr>
@@ -4252,7 +3790,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AC8" authorId="1" shapeId="0" xr:uid="{ED48764E-0DE6-474B-99F1-B7FA628A3AC9}">
+    <comment ref="AA8" authorId="1" shapeId="0" xr:uid="{ED48764E-0DE6-474B-99F1-B7FA628A3AC9}">
       <text>
         <r>
           <rPr>
@@ -4285,7 +3823,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AD8" authorId="1" shapeId="0" xr:uid="{0AB7DD1B-25CB-474D-B9DE-C96B24A9100E}">
+    <comment ref="AB8" authorId="1" shapeId="0" xr:uid="{0AB7DD1B-25CB-474D-B9DE-C96B24A9100E}">
       <text>
         <r>
           <rPr>
@@ -4323,7 +3861,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="44">
   <si>
     <t>Case</t>
   </si>
@@ -4374,12 +3912,6 @@
   </si>
   <si>
     <t>e_qo_M</t>
-  </si>
-  <si>
-    <t>t_own_orig</t>
-  </si>
-  <si>
-    <t>t_own_star</t>
   </si>
   <si>
     <t>t_life_orig</t>
@@ -4538,12 +4070,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="4" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="3" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="3" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4875,13 +4409,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37C61C24-5EEE-2E43-8BFA-CC2DA9B61850}">
-  <dimension ref="A1:AD8"/>
+  <dimension ref="A1:AB8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="S2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="P2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="Y10" sqref="Y10"/>
+      <selection pane="bottomRight" activeCell="W3" sqref="W3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4896,13 +4430,13 @@
     <col min="16" max="16" width="19" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="11.83203125" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="23" max="24" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="25" max="26" width="13.6640625" customWidth="1"/>
+    <col min="21" max="22" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="23" max="24" width="13.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -4914,16 +4448,16 @@
         <v>2</v>
       </c>
       <c r="E1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="G1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="H1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="I1" t="s">
         <v>10</v>
@@ -4932,10 +4466,10 @@
         <v>3</v>
       </c>
       <c r="K1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="L1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="M1" t="s">
         <v>15</v>
@@ -4944,10 +4478,10 @@
         <v>16</v>
       </c>
       <c r="O1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="P1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="Q1" t="s">
         <v>4</v>
@@ -4959,13 +4493,13 @@
         <v>11</v>
       </c>
       <c r="T1" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="U1" t="s">
-        <v>12</v>
+        <v>40</v>
       </c>
       <c r="V1" t="s">
-        <v>18</v>
+        <v>41</v>
       </c>
       <c r="W1" t="s">
         <v>42</v>
@@ -4974,30 +4508,24 @@
         <v>43</v>
       </c>
       <c r="Y1" t="s">
-        <v>44</v>
+        <v>13</v>
       </c>
       <c r="Z1" t="s">
-        <v>45</v>
+        <v>17</v>
       </c>
       <c r="AA1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="AB1" t="s">
-        <v>19</v>
-      </c>
-      <c r="AC1" t="s">
-        <v>14</v>
-      </c>
-      <c r="AD1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>22</v>
-      </c>
       <c r="B2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C2" t="s">
         <v>8</v>
@@ -5009,10 +4537,10 @@
         <v>0.03</v>
       </c>
       <c r="F2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="H2">
         <v>3.6</v>
@@ -5051,45 +4579,39 @@
         <v>10</v>
       </c>
       <c r="T2">
-        <v>1.8</v>
+        <v>1</v>
       </c>
       <c r="U2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="V2">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="W2">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="X2">
         <v>0</v>
       </c>
       <c r="Y2">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="Z2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA2">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="AB2">
         <v>1</v>
       </c>
-      <c r="AC2">
-        <v>1</v>
-      </c>
-      <c r="AD2">
-        <v>1</v>
-      </c>
     </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C3" t="s">
         <v>6</v>
@@ -5101,10 +4623,10 @@
         <v>0.03</v>
       </c>
       <c r="F3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="G3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="H3">
         <v>126.62163000000001</v>
@@ -5139,49 +4661,43 @@
       <c r="R3" s="2">
         <v>27929.825550000001</v>
       </c>
-      <c r="S3">
-        <v>33446.43</v>
-      </c>
-      <c r="T3">
-        <v>7</v>
-      </c>
-      <c r="U3" s="1">
-        <v>33037.919999999998</v>
-      </c>
-      <c r="V3">
-        <v>7</v>
-      </c>
-      <c r="W3" s="3">
-        <v>5000</v>
-      </c>
-      <c r="X3" s="3">
-        <v>5000</v>
-      </c>
-      <c r="Y3" s="4">
+      <c r="S3" s="5">
+        <v>35460</v>
+      </c>
+      <c r="T3" s="6">
+        <v>35255</v>
+      </c>
+      <c r="U3" s="3">
+        <v>5050</v>
+      </c>
+      <c r="V3" s="3">
+        <v>4779</v>
+      </c>
+      <c r="W3" s="4">
         <v>-300</v>
       </c>
-      <c r="Z3" s="4">
+      <c r="X3" s="4">
         <v>-300</v>
       </c>
+      <c r="Y3">
+        <v>34000</v>
+      </c>
+      <c r="Z3">
+        <v>14</v>
+      </c>
       <c r="AA3">
-        <v>34000</v>
+        <v>40000</v>
       </c>
       <c r="AB3">
         <v>14</v>
       </c>
-      <c r="AC3">
-        <v>40000</v>
-      </c>
-      <c r="AD3">
-        <v>14</v>
-      </c>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" t="s">
         <v>22</v>
-      </c>
-      <c r="B4" t="s">
-        <v>24</v>
       </c>
       <c r="C4" t="s">
         <v>8</v>
@@ -5193,10 +4709,10 @@
         <v>0.03</v>
       </c>
       <c r="F4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="H4">
         <v>3.6</v>
@@ -5235,13 +4751,13 @@
         <v>1.88</v>
       </c>
       <c r="T4">
-        <v>1.8</v>
+        <v>1.21</v>
       </c>
       <c r="U4">
-        <v>1.21</v>
+        <v>0</v>
       </c>
       <c r="V4">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="W4">
         <v>0</v>
@@ -5250,30 +4766,24 @@
         <v>0</v>
       </c>
       <c r="Y4">
-        <v>0</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="Z4">
-        <v>0</v>
+        <v>1.8</v>
       </c>
       <c r="AA4">
-        <v>2.2000000000000002</v>
+        <v>6.5</v>
       </c>
       <c r="AB4">
-        <v>1.8</v>
-      </c>
-      <c r="AC4">
-        <v>6.5</v>
-      </c>
-      <c r="AD4">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C5" t="s">
         <v>6</v>
@@ -5285,10 +4795,10 @@
         <v>0.03</v>
       </c>
       <c r="F5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="G5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="H5">
         <v>126.62163000000001</v>
@@ -5326,46 +4836,40 @@
       <c r="S5">
         <v>33446.43</v>
       </c>
-      <c r="T5">
-        <v>7</v>
-      </c>
-      <c r="U5" s="1">
+      <c r="T5" s="1">
         <v>33037.919999999998</v>
       </c>
-      <c r="V5">
-        <v>7</v>
-      </c>
-      <c r="W5" s="2">
+      <c r="U5" s="2">
         <v>2730.84854</v>
       </c>
-      <c r="X5" s="2">
+      <c r="V5" s="2">
         <v>2709.6940300000001</v>
       </c>
+      <c r="W5">
+        <v>0</v>
+      </c>
+      <c r="X5">
+        <v>0</v>
+      </c>
       <c r="Y5">
-        <v>0</v>
+        <v>34000</v>
       </c>
       <c r="Z5">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="AA5">
-        <v>34000</v>
+        <v>40000</v>
       </c>
       <c r="AB5">
         <v>14</v>
       </c>
-      <c r="AC5">
-        <v>40000</v>
-      </c>
-      <c r="AD5">
-        <v>14</v>
-      </c>
     </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B6" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C6" t="s">
         <v>8</v>
@@ -5377,10 +4881,10 @@
         <v>0.03</v>
       </c>
       <c r="F6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G6" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="H6">
         <v>3.6</v>
@@ -5419,13 +4923,13 @@
         <v>1.88</v>
       </c>
       <c r="T6">
-        <v>1.8</v>
+        <v>1.21</v>
       </c>
       <c r="U6">
-        <v>1.21</v>
+        <v>0</v>
       </c>
       <c r="V6">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="W6">
         <v>0</v>
@@ -5434,30 +4938,24 @@
         <v>0</v>
       </c>
       <c r="Y6">
-        <v>0</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="Z6">
-        <v>0</v>
+        <v>1.8</v>
       </c>
       <c r="AA6">
-        <v>2.2000000000000002</v>
+        <v>6.5</v>
       </c>
       <c r="AB6">
-        <v>1.8</v>
-      </c>
-      <c r="AC6">
-        <v>6.5</v>
-      </c>
-      <c r="AD6">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B7" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C7" t="s">
         <v>6</v>
@@ -5469,10 +4967,10 @@
         <v>0.03</v>
       </c>
       <c r="F7" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="G7" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="H7">
         <v>126.62163000000001</v>
@@ -5510,46 +5008,40 @@
       <c r="S7">
         <v>33446.43</v>
       </c>
-      <c r="T7">
-        <v>7</v>
-      </c>
-      <c r="U7" s="1">
+      <c r="T7" s="1">
         <v>33037.919999999998</v>
       </c>
-      <c r="V7">
-        <v>7</v>
-      </c>
-      <c r="W7" s="2">
+      <c r="U7" s="2">
         <v>2730.84854</v>
       </c>
-      <c r="X7" s="2">
+      <c r="V7" s="2">
         <v>2709.6940300000001</v>
       </c>
+      <c r="W7">
+        <v>0</v>
+      </c>
+      <c r="X7">
+        <v>0</v>
+      </c>
       <c r="Y7">
-        <v>0</v>
+        <v>34000</v>
       </c>
       <c r="Z7">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="AA7">
-        <v>34000</v>
+        <v>40000</v>
       </c>
       <c r="AB7">
         <v>14</v>
       </c>
-      <c r="AC7">
-        <v>40000</v>
-      </c>
-      <c r="AD7">
-        <v>14</v>
-      </c>
     </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B8" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C8" t="s">
         <v>8</v>
@@ -5561,10 +5053,10 @@
         <v>0.03</v>
       </c>
       <c r="F8" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G8" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="H8">
         <v>3.6</v>
@@ -5603,13 +5095,13 @@
         <v>1.88</v>
       </c>
       <c r="T8">
-        <v>1.8</v>
+        <v>1.21</v>
       </c>
       <c r="U8">
-        <v>1.21</v>
+        <v>0</v>
       </c>
       <c r="V8">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="W8">
         <v>0</v>
@@ -5618,21 +5110,15 @@
         <v>0</v>
       </c>
       <c r="Y8">
-        <v>0</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="Z8">
-        <v>0</v>
+        <v>1.8</v>
       </c>
       <c r="AA8">
-        <v>2.2000000000000002</v>
+        <v>6.5</v>
       </c>
       <c r="AB8">
-        <v>1.8</v>
-      </c>
-      <c r="AC8">
-        <v>6.5</v>
-      </c>
-      <c r="AD8">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add section on elasticity
</commit_message>
<xml_diff>
--- a/data/eeu_data.xlsx
+++ b/data/eeu_data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11027"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mkh2/github/ReboundPaper2022/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F3EB564-254E-7C4B-B4B2-145E794993FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{084FBDCB-AFDD-974C-9557-5603718743C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="28800" windowHeight="9080" xr2:uid="{7964B245-1BB5-784B-946F-34F7FEF70238}"/>
   </bookViews>
@@ -2695,7 +2695,6 @@
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
-            <scheme val="minor"/>
           </rPr>
           <t>$</t>
         </r>
@@ -3956,6 +3955,501 @@
       </text>
     </comment>
     <comment ref="AB8" authorId="1" shapeId="0" xr:uid="{0AB7DD1B-25CB-474D-B9DE-C96B24A9100E}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matthew Heun:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>years</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H9" authorId="1" shapeId="0" xr:uid="{3D8F4127-6F42-C544-9F7F-E800072C6999}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matthew Heun:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>MJ/kW-hr</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I9" authorId="1" shapeId="0" xr:uid="{820F2D03-D690-EA4D-BFEC-BD16CBF3E8E2}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matthew Heun:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>MJ/$</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K9" authorId="1" shapeId="0" xr:uid="{33C8D43C-1DF4-5F44-8BDE-AD09056A8C35}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matthew Heun:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>$/kW-hr</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="O9" authorId="1" shapeId="0" xr:uid="{2FCBBCDE-CCFF-5948-BC50-897A0B9985B5}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matthew Heun:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>lm-hr/kW-hr</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="P9" authorId="1" shapeId="0" xr:uid="{07F4116C-2678-234A-912C-266CABEFA724}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matthew Heun:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>lm-hr/kW-hr</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="Q9" authorId="1" shapeId="0" xr:uid="{4CA0D134-7BC1-054C-9B34-26CE876937C3}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matthew Heun:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Lm-hr/yr</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="R9" authorId="1" shapeId="0" xr:uid="{7260F56F-7AD9-6946-BDDF-9AFCB45DCC0D}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matthew Heun:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>$/year</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="S9" authorId="1" shapeId="0" xr:uid="{A8FC70F8-BF46-8440-97DB-A5583A6792EF}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matthew Heun:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>$</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="T9" authorId="1" shapeId="0" xr:uid="{DB1B9D45-A9F5-C340-AE3D-4644D848636A}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matthew Heun:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>$</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="U9" authorId="1" shapeId="0" xr:uid="{7DDEDDF5-B10E-354D-80A4-18E8EDA82158}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matthew Heun:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>$/year</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="V9" authorId="1" shapeId="0" xr:uid="{AE541944-D791-B64C-A27A-E0592D626540}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matthew Heun:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>$/year</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="Y9" authorId="1" shapeId="0" xr:uid="{8ACCDA0E-5F0D-F24D-BF66-E4FC4398D926}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matthew Heun:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>MJ</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="Z9" authorId="1" shapeId="0" xr:uid="{46069FB5-A89D-F247-BF9E-7B80252A7FDC}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matthew Heun:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>years</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AA9" authorId="1" shapeId="0" xr:uid="{2B96A9B4-0751-AF44-B9A7-0774916C37A8}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matthew Heun:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>MJ</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AB9" authorId="1" shapeId="0" xr:uid="{ACC29C9A-9EE8-674C-AC47-E2602C842048}">
       <text>
         <r>
           <rPr>
@@ -3993,7 +4487,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="45">
   <si>
     <t>Case</t>
   </si>
@@ -4126,6 +4620,9 @@
   <si>
     <t>e_qg_M</t>
   </si>
+  <si>
+    <t>Lamp (k = 3, eps = -0.128)</t>
+  </si>
 </sst>
 </file>
 
@@ -4134,7 +4631,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.00000"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -4161,13 +4658,6 @@
       <color rgb="FF000000"/>
       <name val="Tahoma"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
@@ -4541,13 +5031,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37C61C24-5EEE-2E43-8BFA-CC2DA9B61850}">
-  <dimension ref="A1:AB8"/>
+  <dimension ref="A1:AB9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="Q2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="N1" sqref="N1"/>
+      <selection pane="bottomRight" activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5254,6 +5744,92 @@
         <v>10</v>
       </c>
     </row>
+    <row r="9" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" t="s">
+        <v>44</v>
+      </c>
+      <c r="C9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9">
+        <v>0.03</v>
+      </c>
+      <c r="F9" t="s">
+        <v>36</v>
+      </c>
+      <c r="G9" t="s">
+        <v>37</v>
+      </c>
+      <c r="H9">
+        <v>3.6</v>
+      </c>
+      <c r="I9">
+        <v>3.2380660967337498</v>
+      </c>
+      <c r="J9">
+        <v>3</v>
+      </c>
+      <c r="K9">
+        <v>0.12870000000000001</v>
+      </c>
+      <c r="L9">
+        <v>-0.128</v>
+      </c>
+      <c r="M9">
+        <v>1</v>
+      </c>
+      <c r="N9">
+        <v>1</v>
+      </c>
+      <c r="O9" s="1">
+        <v>8833.3333333333303</v>
+      </c>
+      <c r="P9">
+        <v>81800</v>
+      </c>
+      <c r="Q9">
+        <v>580350</v>
+      </c>
+      <c r="R9" s="2">
+        <v>27929.825550000001</v>
+      </c>
+      <c r="S9">
+        <v>1.88</v>
+      </c>
+      <c r="T9">
+        <v>1.21</v>
+      </c>
+      <c r="U9">
+        <v>0</v>
+      </c>
+      <c r="V9">
+        <v>0</v>
+      </c>
+      <c r="W9">
+        <v>0</v>
+      </c>
+      <c r="X9">
+        <v>0</v>
+      </c>
+      <c r="Y9">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="Z9">
+        <v>1.8</v>
+      </c>
+      <c r="AA9">
+        <v>6.5</v>
+      </c>
+      <c r="AB9">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
Reacting to PEB comments.
</commit_message>
<xml_diff>
--- a/data/eeu_data.xlsx
+++ b/data/eeu_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mkh2/github/ReboundPaper2022/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{084FBDCB-AFDD-974C-9557-5603718743C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D52471A-C0E6-FF47-9546-02CC24D32ADE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="28800" windowHeight="9080" xr2:uid="{7964B245-1BB5-784B-946F-34F7FEF70238}"/>
   </bookViews>
@@ -4482,12 +4482,507 @@
         </r>
       </text>
     </comment>
+    <comment ref="H10" authorId="1" shapeId="0" xr:uid="{8EC233ED-EE7D-004D-B070-80080110226B}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matthew Heun:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>MJ/kW-hr</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I10" authorId="1" shapeId="0" xr:uid="{C1A351CE-EABB-A141-AC2E-E9279410433E}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matthew Heun:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>MJ/$</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K10" authorId="1" shapeId="0" xr:uid="{D4DD8415-B01C-0143-A865-8F3BEF14E5C8}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matthew Heun:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>$/kW-hr</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="O10" authorId="1" shapeId="0" xr:uid="{5C4E5F44-3350-2B47-87A2-A671A5783F63}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matthew Heun:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>lm-hr/kW-hr</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="P10" authorId="1" shapeId="0" xr:uid="{E4ACD8F0-D25F-0141-B5B9-FC0D9089B3A2}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matthew Heun:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>lm-hr/kW-hr</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="Q10" authorId="1" shapeId="0" xr:uid="{931828A4-642B-B34C-8593-4FC7DBE044EE}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matthew Heun:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Lm-hr/yr</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="R10" authorId="1" shapeId="0" xr:uid="{A76120FB-CCDC-DA4F-A5E1-9682CB7AE416}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matthew Heun:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>$/year</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="S10" authorId="1" shapeId="0" xr:uid="{3D8706B4-3890-6F4D-9A30-4B9DA8DBE48B}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matthew Heun:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>$</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="T10" authorId="1" shapeId="0" xr:uid="{D2EDE476-2402-0A42-99D7-0DB7C10ED1C5}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matthew Heun:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>$</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="U10" authorId="1" shapeId="0" xr:uid="{11AEB694-85D2-5242-A27B-476462031F2B}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matthew Heun:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>$/year</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="V10" authorId="1" shapeId="0" xr:uid="{221B36BB-4EEA-F744-B654-AB8B674030C5}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matthew Heun:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>$/year</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="Y10" authorId="1" shapeId="0" xr:uid="{C329FC96-06C7-9D45-ACD6-3843902015A8}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matthew Heun:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>MJ</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="Z10" authorId="1" shapeId="0" xr:uid="{28C1771B-46D1-3942-9223-3AFCD6FFE7B0}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matthew Heun:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>years</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AA10" authorId="1" shapeId="0" xr:uid="{B2629AA8-9142-C34D-B16F-D0A571C61E2C}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matthew Heun:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>MJ</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AB10" authorId="1" shapeId="0" xr:uid="{FC219151-1F58-6C48-B9FF-64FB0E9C2758}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matthew Heun:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>years</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="46">
   <si>
     <t>Case</t>
   </si>
@@ -4622,6 +5117,9 @@
   </si>
   <si>
     <t>Lamp (k = 3, eps = -0.128)</t>
+  </si>
+  <si>
+    <t>Lamp (k = 3, eps = -0.6)</t>
   </si>
 </sst>
 </file>
@@ -5031,13 +5529,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37C61C24-5EEE-2E43-8BFA-CC2DA9B61850}">
-  <dimension ref="A1:AB9"/>
+  <dimension ref="A1:AB10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="Q2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B9" sqref="B9"/>
+      <selection pane="bottomRight" activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5830,6 +6328,92 @@
         <v>10</v>
       </c>
     </row>
+    <row r="10" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" t="s">
+        <v>45</v>
+      </c>
+      <c r="C10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10">
+        <v>0.03</v>
+      </c>
+      <c r="F10" t="s">
+        <v>36</v>
+      </c>
+      <c r="G10" t="s">
+        <v>37</v>
+      </c>
+      <c r="H10">
+        <v>3.6</v>
+      </c>
+      <c r="I10">
+        <v>3.2380660967337498</v>
+      </c>
+      <c r="J10">
+        <v>3</v>
+      </c>
+      <c r="K10">
+        <v>0.12870000000000001</v>
+      </c>
+      <c r="L10">
+        <v>-0.6</v>
+      </c>
+      <c r="M10">
+        <v>1</v>
+      </c>
+      <c r="N10">
+        <v>1</v>
+      </c>
+      <c r="O10" s="1">
+        <v>8833.3333333333303</v>
+      </c>
+      <c r="P10">
+        <v>81800</v>
+      </c>
+      <c r="Q10">
+        <v>580350</v>
+      </c>
+      <c r="R10" s="2">
+        <v>27929.825550000001</v>
+      </c>
+      <c r="S10">
+        <v>1.88</v>
+      </c>
+      <c r="T10">
+        <v>1.21</v>
+      </c>
+      <c r="U10">
+        <v>0</v>
+      </c>
+      <c r="V10">
+        <v>0</v>
+      </c>
+      <c r="W10">
+        <v>0</v>
+      </c>
+      <c r="X10">
+        <v>0</v>
+      </c>
+      <c r="Y10">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="Z10">
+        <v>1.8</v>
+      </c>
+      <c r="AA10">
+        <v>6.5</v>
+      </c>
+      <c r="AB10">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>